<commit_message>
added rename logic and basic error handling
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcerr\Documents\vscodeprojects\renombrarFotos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLAUDIA\Desktop\DavidC\vsprojects\renombrarFotos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42A6F725-261A-46D1-B5B3-9914D8B4D84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D568981-EF36-4FB4-9F52-6B6015E9F8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{701EF7F7-DC50-48C4-B21F-F97BF3F571E7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{701EF7F7-DC50-48C4-B21F-F97BF3F571E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>M6000_597_V2_Q125_FLATSQUARE.jpg</t>
   </si>
@@ -92,7 +90,10 @@
     <t>M6000_597</t>
   </si>
   <si>
-    <t>M6000_V56</t>
+    <t>L8258_T11</t>
+  </si>
+  <si>
+    <t>C8161_X11</t>
   </si>
 </sst>
 </file>
@@ -470,12 +471,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -483,7 +484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -491,77 +492,80 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>16</v>
       </c>

</xml_diff>